<commit_message>
ran wb 23 feb emma looking good
</commit_message>
<xml_diff>
--- a/data/newrnet-chemistry/RI23_endmemeber_manual_sort.xlsx
+++ b/data/newrnet-chemistry/RI23_endmemeber_manual_sort.xlsx
@@ -947,8 +947,8 @@
   </sheetPr>
   <dimension ref="A1:AD139"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:B139"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A77" activeCellId="0" sqref="77:77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10240,7 +10240,7 @@
   <dimension ref="A1:AD16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="1" sqref="B1:B139 C18"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="1" sqref="77:77 C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11301,7 +11301,7 @@
   <dimension ref="A1:AD8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="B1:B139 A3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="77:77 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11863,7 +11863,7 @@
   <dimension ref="A1:AD19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="B1:B139 D17"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="77:77 D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>